<commit_message>
memperbaiki fungsi download logbook yang menghasilkan file halusinasi
</commit_message>
<xml_diff>
--- a/server/templates/logbook.xlsx
+++ b/server/templates/logbook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADAC8DE-87D9-4618-957E-BB22DE199764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A34D4D3-FE49-4732-B175-8BBC9A1A1626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="3540" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logbook" sheetId="17" r:id="rId1"/>
@@ -513,6 +513,15 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,21 +546,18 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,12 +566,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -888,61 +888,61 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="18" width="13.453125" customWidth="1"/>
-    <col min="19" max="19" width="13.81640625" customWidth="1"/>
+    <col min="3" max="18" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:19" ht="20.25">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-    </row>
-    <row r="2" spans="1:19" ht="20">
-      <c r="A2" s="49" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+    </row>
+    <row r="2" spans="1:19" ht="20.25">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-    </row>
-    <row r="3" spans="1:19" ht="20.5">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+    </row>
+    <row r="3" spans="1:19" ht="20.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -963,7 +963,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:19" ht="20.5">
+    <row r="4" spans="1:19" ht="20.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -992,7 +992,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:19" ht="20.5">
+    <row r="5" spans="1:19" ht="20.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="R5" s="7"/>
       <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="20.5">
+    <row r="6" spans="1:19" ht="20.25">
       <c r="A6" s="45" t="s">
         <v>28</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:19" ht="20.5">
+    <row r="7" spans="1:19" ht="20.25">
       <c r="A7" s="45" t="s">
         <v>30</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="R7" s="10"/>
       <c r="S7" s="11"/>
     </row>
-    <row r="8" spans="1:19" ht="20.5">
+    <row r="8" spans="1:19" ht="20.25">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="R8" s="10"/>
       <c r="S8" s="11"/>
     </row>
-    <row r="9" spans="1:19" ht="15.5">
+    <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="12"/>
       <c r="B9" s="1"/>
       <c r="C9" s="13"/>
@@ -1122,37 +1122,37 @@
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" ht="16.5">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="R10" s="59"/>
       <c r="S10" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="16.5">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="17">
         <v>1</v>
       </c>
@@ -1204,8 +1204,8 @@
       <c r="S11" s="61"/>
     </row>
     <row r="12" spans="1:19" ht="16.5">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="17" t="s">
         <v>18</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="S12" s="61"/>
     </row>
-    <row r="13" spans="1:19" ht="38.5" customHeight="1">
+    <row r="13" spans="1:19" ht="38.450000000000003" customHeight="1">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="20"/>
@@ -1269,15 +1269,15 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="65"/>
+      <c r="M13" s="50"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="21"/>
-      <c r="S13" s="62"/>
-    </row>
-    <row r="14" spans="1:19" ht="38.5" customHeight="1">
+      <c r="S13" s="64"/>
+    </row>
+    <row r="14" spans="1:19" ht="38.450000000000003" customHeight="1">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
@@ -1290,19 +1290,19 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="66"/>
+      <c r="M14" s="51"/>
       <c r="N14" s="47"/>
       <c r="O14" s="20"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="21"/>
       <c r="R14" s="21"/>
-      <c r="S14" s="63"/>
+      <c r="S14" s="65"/>
     </row>
     <row r="15" spans="1:19" ht="16.5">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="58"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -1318,10 +1318,10 @@
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="64"/>
-    </row>
-    <row r="16" spans="1:19" ht="15.5">
+      <c r="R15" s="49"/>
+      <c r="S15" s="66"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
@@ -1344,7 +1344,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="26"/>
     </row>
-    <row r="17" spans="1:19" ht="15.5">
+    <row r="17" spans="1:19" ht="15.75">
       <c r="A17" s="23"/>
       <c r="B17" s="24"/>
       <c r="C17" s="25"/>
@@ -1365,7 +1365,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="26"/>
     </row>
-    <row r="18" spans="1:19" ht="15.5">
+    <row r="18" spans="1:19" ht="15.75">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
@@ -1386,7 +1386,7 @@
       <c r="R18" s="25"/>
       <c r="S18" s="26"/>
     </row>
-    <row r="19" spans="1:19" ht="15.5">
+    <row r="19" spans="1:19" ht="15.75">
       <c r="A19" s="27"/>
       <c r="B19" s="28"/>
       <c r="C19" s="14"/>
@@ -1409,7 +1409,7 @@
       <c r="R19" s="27"/>
       <c r="S19" s="28"/>
     </row>
-    <row r="20" spans="1:19" ht="15.5">
+    <row r="20" spans="1:19" ht="15.75">
       <c r="A20" s="27"/>
       <c r="B20" s="28" t="s">
         <v>21</v>
@@ -1431,7 +1431,7 @@
       <c r="R20" s="27"/>
       <c r="S20" s="28"/>
     </row>
-    <row r="21" spans="1:19" ht="15.5">
+    <row r="21" spans="1:19" ht="15.75">
       <c r="A21" s="27"/>
       <c r="B21" s="28" t="s">
         <v>22</v>
@@ -1456,7 +1456,7 @@
       <c r="R21" s="27"/>
       <c r="S21" s="28"/>
     </row>
-    <row r="22" spans="1:19" ht="15.5">
+    <row r="22" spans="1:19" ht="15.75">
       <c r="A22" s="27"/>
       <c r="B22" s="28"/>
       <c r="C22" s="14"/>
@@ -1477,7 +1477,7 @@
       <c r="R22" s="27"/>
       <c r="S22" s="28"/>
     </row>
-    <row r="23" spans="1:19" ht="15.5">
+    <row r="23" spans="1:19" ht="15.75">
       <c r="A23" s="27"/>
       <c r="B23" s="28"/>
       <c r="C23" s="14"/>
@@ -1498,7 +1498,7 @@
       <c r="R23" s="27"/>
       <c r="S23" s="28"/>
     </row>
-    <row r="24" spans="1:19" ht="15.5">
+    <row r="24" spans="1:19" ht="15.75">
       <c r="A24" s="27"/>
       <c r="B24" s="28"/>
       <c r="C24" s="14"/>
@@ -1519,7 +1519,7 @@
       <c r="R24" s="27"/>
       <c r="S24" s="28"/>
     </row>
-    <row r="25" spans="1:19" ht="15.5">
+    <row r="25" spans="1:19" ht="15.75">
       <c r="A25" s="30"/>
       <c r="B25" s="31"/>
       <c r="C25" s="30"/>
@@ -1540,7 +1540,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="1:19" ht="15.5">
+    <row r="26" spans="1:19" ht="15.75">
       <c r="A26" s="30"/>
       <c r="B26" s="31"/>
       <c r="C26" s="30"/>
@@ -1561,7 +1561,7 @@
       <c r="R26" s="31"/>
       <c r="S26" s="31"/>
     </row>
-    <row r="27" spans="1:19" ht="15.5">
+    <row r="27" spans="1:19" ht="15.75">
       <c r="A27" s="14"/>
       <c r="B27" s="33" t="s">
         <v>24</v>
@@ -1586,7 +1586,7 @@
       <c r="R27" s="34"/>
       <c r="S27" s="33"/>
     </row>
-    <row r="28" spans="1:19" ht="15.5">
+    <row r="28" spans="1:19" ht="15.75">
       <c r="A28" s="35"/>
       <c r="B28" s="36" t="s">
         <v>26</v>
@@ -1611,7 +1611,7 @@
       <c r="R28" s="35"/>
       <c r="S28" s="38"/>
     </row>
-    <row r="29" spans="1:19" ht="15.5">
+    <row r="29" spans="1:19" ht="15.75">
       <c r="A29" s="41"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1634,14 +1634,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="S13:S15"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:R10"/>
     <mergeCell ref="S10:S12"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="S13:S15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>